<commit_message>
fixed bug with strftime
</commit_message>
<xml_diff>
--- a/vis/people_coloured_projects.xlsx
+++ b/vis/people_coloured_projects.xlsx
@@ -397,19 +397,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBF174"/>
+        <fgColor rgb="FFE0B5E0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF876B8"/>
+        <fgColor rgb="FF86E3B6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF87CF7B"/>
+        <fgColor rgb="FF9EF7F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,193 +421,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5C76F8"/>
+        <fgColor rgb="FF5A855C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC2DBEA"/>
+        <fgColor rgb="FFFC92AD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAC9A83"/>
+        <fgColor rgb="FFFDD695"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEA5F83"/>
+        <fgColor rgb="FF7C62C5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5DF19D"/>
+        <fgColor rgb="FF57F8A3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD2B76A"/>
+        <fgColor rgb="FFB28E9D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5EBBDD"/>
+        <fgColor rgb="FFD873D7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF97F8D3"/>
+        <fgColor rgb="FF7296FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6EEDFF"/>
+        <fgColor rgb="FF65D286"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBEA5CB"/>
+        <fgColor rgb="FFE0EFAE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFAD060"/>
+        <fgColor rgb="FFA87FEB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF9C7D9"/>
+        <fgColor rgb="FF91D057"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF655B7A"/>
+        <fgColor rgb="FF585B88"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE293F3"/>
+        <fgColor rgb="FFAFA25F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1FEBB"/>
+        <fgColor rgb="FFDB7487"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBA835B"/>
+        <fgColor rgb="FF905863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFC62FB"/>
+        <fgColor rgb="FFAEFE7F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB0F656"/>
+        <fgColor rgb="FFFA55F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD69CA0"/>
+        <fgColor rgb="FFBED7CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAD78FD"/>
+        <fgColor rgb="FFFEF5ED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC262C9"/>
+        <fgColor rgb="FF7196A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF876457"/>
+        <fgColor rgb="FF58D0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFADE496"/>
+        <fgColor rgb="FFEA575C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB581AE"/>
+        <fgColor rgb="FF5884CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8C9FEE"/>
+        <fgColor rgb="FFFDAE73"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6CA462"/>
+        <fgColor rgb="FF6058F9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8E6D93"/>
+        <fgColor rgb="FF88A8DA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF588ABD"/>
+        <fgColor rgb="FFC4C197"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6CF561"/>
+        <fgColor rgb="FFEDDB5A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7BA9A9"/>
+        <fgColor rgb="FFB556BF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8056E2"/>
+        <fgColor rgb="FFB5BAFC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA0C0BF"/>
+        <fgColor rgb="FF5CEA5D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>

<commit_message>
started cleaning up visualise_forecast  functions
</commit_message>
<xml_diff>
--- a/vis/people_coloured_projects.xlsx
+++ b/vis/people_coloured_projects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="119">
   <si>
     <t>Nov-2018</t>
   </si>
@@ -172,25 +172,25 @@
     <t>3rd</t>
   </si>
   <si>
-    <t>AIDA (0.8)</t>
-  </si>
-  <si>
-    <t>Living With Machines (0.8)</t>
-  </si>
-  <si>
-    <t>NATS (0.4)</t>
-  </si>
-  <si>
-    <t>BA (IAG) (0.4)</t>
-  </si>
-  <si>
-    <t>Living With Machines (0.4)</t>
-  </si>
-  <si>
-    <t>AIDA (0.4)</t>
-  </si>
-  <si>
-    <t>Nocell (0.4)</t>
+    <t>AIDA (1.0)</t>
+  </si>
+  <si>
+    <t>Living With Machines (1.0)</t>
+  </si>
+  <si>
+    <t>NATS (0.5)</t>
+  </si>
+  <si>
+    <t>BA (IAG) (0.5)</t>
+  </si>
+  <si>
+    <t>Living With Machines (0.5)</t>
+  </si>
+  <si>
+    <t>AIDA (0.5)</t>
+  </si>
+  <si>
+    <t>Nocell (0.5)</t>
   </si>
   <si>
     <t>BA (IAG) (0.2)</t>
@@ -199,142 +199,148 @@
     <t>AIDA (0.2)</t>
   </si>
   <si>
-    <t>SPF TPS Theme Management (0.5)</t>
+    <t>SPF TPS Theme Management (0.6)</t>
   </si>
   <si>
     <t>Training delivery (0.1)</t>
   </si>
   <si>
+    <t>Safe Haven (0.5)</t>
+  </si>
+  <si>
+    <t>Misinformation (0.5)</t>
+  </si>
+  <si>
+    <t>The Turing Way (0.5)</t>
+  </si>
+  <si>
+    <t>AI for City Planning (0.5)</t>
+  </si>
+  <si>
+    <t>Team management (0.5)</t>
+  </si>
+  <si>
+    <t>Biobank algorithm (0.6)</t>
+  </si>
+  <si>
+    <t>Parallel Monte Carlo (0.1)</t>
+  </si>
+  <si>
+    <t>Fitbit classification (0.1)</t>
+  </si>
+  <si>
+    <t>Crypto Federated Learning (SHEEP) (0.5)</t>
+  </si>
+  <si>
+    <t>Maru (0.5)</t>
+  </si>
+  <si>
+    <t>Sargasso (Intel Sparse) (0.5)</t>
+  </si>
+  <si>
+    <t>Crypto Federated Learning (SHEEP) (0.2)</t>
+  </si>
+  <si>
+    <t>BA (IAG) (1.0)</t>
+  </si>
+  <si>
+    <t>AIDA-Lloyds (0.5)</t>
+  </si>
+  <si>
+    <t>DetectorChecker (0.5)</t>
+  </si>
+  <si>
+    <t>Knowledge Flows (0.5)</t>
+  </si>
+  <si>
+    <t>Probabilistic FEM (0.5)</t>
+  </si>
+  <si>
+    <t>GUARD (0.4)</t>
+  </si>
+  <si>
+    <t>AIDA (0.1)</t>
+  </si>
+  <si>
+    <t>Living With Machines (0.1) / Safe Haven (0.1)</t>
+  </si>
+  <si>
+    <t>ALOGIT Python (0.4)</t>
+  </si>
+  <si>
+    <t>Safe Haven (0.8)</t>
+  </si>
+  <si>
+    <t>Team management (0.0)</t>
+  </si>
+  <si>
+    <t>Misinformation (0.0)</t>
+  </si>
+  <si>
+    <t>Parallel Monte Carlo (0.5)</t>
+  </si>
+  <si>
+    <t>Fitbit classification (0.5)</t>
+  </si>
+  <si>
+    <t>Maru (0.6)</t>
+  </si>
+  <si>
+    <t>Data Science Benchmarking (0.5)</t>
+  </si>
+  <si>
+    <t>UQM^3 (0.4)</t>
+  </si>
+  <si>
+    <t>CWTS - Leiden (0.2)</t>
+  </si>
+  <si>
+    <t>GUARD (0.2)</t>
+  </si>
+  <si>
+    <t>SPF Learning Machines (0.1)</t>
+  </si>
+  <si>
+    <t>Team management (0.1) / Safe Haven (0.1) / Living With Machines (0.1) / Training delivery (0.1)</t>
+  </si>
+  <si>
     <t>Safe Haven (0.4)</t>
   </si>
   <si>
-    <t>Misinformation (0.4)</t>
-  </si>
-  <si>
-    <t>The Turing Way (0.4)</t>
-  </si>
-  <si>
-    <t>AI for City Planning (0.4)</t>
-  </si>
-  <si>
-    <t>Team management (0.4)</t>
-  </si>
-  <si>
-    <t>Biobank algorithm (0.5)</t>
-  </si>
-  <si>
-    <t>Parallel Monte Carlo (0.1)</t>
-  </si>
-  <si>
-    <t>Fitbit classification (0.1)</t>
-  </si>
-  <si>
-    <t>Crypto Federated Learning (SHEEP) (0.4)</t>
-  </si>
-  <si>
-    <t>Maru (0.4)</t>
-  </si>
-  <si>
-    <t>Sargasso (Intel Sparse) (0.4)</t>
-  </si>
-  <si>
-    <t>Crypto Federated Learning (SHEEP) (0.2)</t>
-  </si>
-  <si>
-    <t>BA (IAG) (0.8)</t>
-  </si>
-  <si>
-    <t>AIDA-Lloyds (0.4)</t>
-  </si>
-  <si>
-    <t>DetectorChecker (0.4)</t>
-  </si>
-  <si>
-    <t>Knowledge Flows (0.4)</t>
-  </si>
-  <si>
-    <t>Probabilistic FEM (0.4)</t>
-  </si>
-  <si>
-    <t>GUARD (0.3)</t>
-  </si>
-  <si>
-    <t>AIDA (0.1)</t>
-  </si>
-  <si>
-    <t>Living With Machines (0.1) / Safe Haven (0.1)</t>
-  </si>
-  <si>
-    <t>ALOGIT Python (0.3)</t>
-  </si>
-  <si>
-    <t>Safe Haven (0.7)</t>
-  </si>
-  <si>
-    <t>Team management (0.0)</t>
-  </si>
-  <si>
-    <t>Misinformation (0.0)</t>
-  </si>
-  <si>
-    <t>Parallel Monte Carlo (0.4)</t>
-  </si>
-  <si>
-    <t>Fitbit classification (0.4)</t>
-  </si>
-  <si>
-    <t>Maru (0.5)</t>
-  </si>
-  <si>
-    <t>Data Science Benchmarking (0.4)</t>
-  </si>
-  <si>
-    <t>UQM^3 (0.3)</t>
-  </si>
-  <si>
-    <t>CWTS - Leiden (0.2)</t>
-  </si>
-  <si>
-    <t>GUARD (0.2)</t>
-  </si>
-  <si>
-    <t>SPF Learning Machines (0.1)</t>
-  </si>
-  <si>
-    <t>Team management (0.1) / Safe Haven (0.1) / Living With Machines (0.1) / Training delivery (0.1)</t>
+    <t>ALOGIT Python (0.5)</t>
+  </si>
+  <si>
+    <t>GUARD (0.5)</t>
+  </si>
+  <si>
+    <t>Team management (0.7)</t>
+  </si>
+  <si>
+    <t>Misinformation (0.3)</t>
+  </si>
+  <si>
+    <t>DS for Sustainable Development (0.5)</t>
+  </si>
+  <si>
+    <t>Nocell (0.6)</t>
+  </si>
+  <si>
+    <t>UQM^3 (0.5)</t>
+  </si>
+  <si>
+    <t>NATS (0.2)</t>
   </si>
   <si>
     <t>Safe Haven (0.3)</t>
   </si>
   <si>
-    <t>ALOGIT Python (0.4)</t>
-  </si>
-  <si>
-    <t>GUARD (0.4)</t>
-  </si>
-  <si>
-    <t>Team management (0.5)</t>
-  </si>
-  <si>
-    <t>Misinformation (0.3)</t>
-  </si>
-  <si>
-    <t>DS for Sustainable Development (0.4)</t>
-  </si>
-  <si>
-    <t>Nocell (0.5)</t>
-  </si>
-  <si>
-    <t>UQM^3 (0.4)</t>
-  </si>
-  <si>
-    <t>NATS (0.2)</t>
-  </si>
-  <si>
-    <t>Team management (0.8)</t>
-  </si>
-  <si>
-    <t>Bayesian Performance Tuning (0.4)</t>
+    <t>Parallel Monte Carlo (0.2)</t>
+  </si>
+  <si>
+    <t>Team management (1.0)</t>
+  </si>
+  <si>
+    <t>Bayesian Performance Tuning (0.5)</t>
   </si>
   <si>
     <t>Team management (0.1)</t>
@@ -343,28 +349,28 @@
     <t>Living With Machines (0.1) / SPF Learning Machines (0.1) / Safe Haven (0.1) / Training delivery (0.1)</t>
   </si>
   <si>
-    <t>NATS (1.0)</t>
-  </si>
-  <si>
-    <t>Uncertainty in Government Modelling (0.5)</t>
+    <t>NATS (1.2)</t>
+  </si>
+  <si>
+    <t>Uncertainty in Government Modelling (0.6)</t>
   </si>
   <si>
     <t>Living With Machines (0.1)</t>
   </si>
   <si>
+    <t>Clean Air (0.5)</t>
+  </si>
+  <si>
+    <t>Streaming healthcare analytics (0.5)</t>
+  </si>
+  <si>
+    <t>Leeds: Lomax, Malleson, Heppenstall (0.6)</t>
+  </si>
+  <si>
+    <t>Urban observatory spatial sampling (0.5)</t>
+  </si>
+  <si>
     <t>Clean Air (0.4)</t>
-  </si>
-  <si>
-    <t>Streaming healthcare analytics (0.4)</t>
-  </si>
-  <si>
-    <t>Leeds: Lomax, Malleson, Heppenstall (0.5)</t>
-  </si>
-  <si>
-    <t>Urban observatory spatial sampling (0.4)</t>
-  </si>
-  <si>
-    <t>Clean Air (0.3)</t>
   </si>
 </sst>
 </file>
@@ -397,19 +403,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE0B5E0"/>
+        <fgColor rgb="FFE6D5B6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF86E3B6"/>
+        <fgColor rgb="FFC5598B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9EF7F8"/>
+        <fgColor rgb="FF9D7856"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,193 +427,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5A855C"/>
+        <fgColor rgb="FF74D0A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFC92AD"/>
+        <fgColor rgb="FFFEEDF9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDD695"/>
+        <fgColor rgb="FFDDFB91"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7C62C5"/>
+        <fgColor rgb="FFB69083"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF57F8A3"/>
+        <fgColor rgb="FFD8869D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB28E9D"/>
+        <fgColor rgb="FFAC72C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD873D7"/>
+        <fgColor rgb="FFCB9DFE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7296FF"/>
+        <fgColor rgb="FF58A75C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF65D286"/>
+        <fgColor rgb="FF9FF1CD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE0EFAE"/>
+        <fgColor rgb="FF9E66FD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA87FEB"/>
+        <fgColor rgb="FFBAC98C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF91D057"/>
+        <fgColor rgb="FF95AAE3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF585B88"/>
+        <fgColor rgb="FF6AFFC1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAFA25F"/>
+        <fgColor rgb="FF7F5664"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDB7487"/>
+        <fgColor rgb="FFF8767C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF905863"/>
+        <fgColor rgb="FFFEE265"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAEFE7F"/>
+        <fgColor rgb="FF729BFB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA55F2"/>
+        <fgColor rgb="FFB3E0FE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBED7CC"/>
+        <fgColor rgb="FF849AB7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFEF5ED"/>
+        <fgColor rgb="FFD3965A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7196A0"/>
+        <fgColor rgb="FF83D857"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF58D0F0"/>
+        <fgColor rgb="FFF0B493"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEA575C"/>
+        <fgColor rgb="FFDC56E2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5884CE"/>
+        <fgColor rgb="FF6460ED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDAE73"/>
+        <fgColor rgb="FF929D70"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6058F9"/>
+        <fgColor rgb="FFE2AAD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF88A8DA"/>
+        <fgColor rgb="FFB4FE5F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC4C197"/>
+        <fgColor rgb="FF5ECEE4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDDB5A"/>
+        <fgColor rgb="FF64FC77"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB556BF"/>
+        <fgColor rgb="FFFF83C2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB5BAFC"/>
+        <fgColor rgb="FF696899"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5CEA5D"/>
+        <fgColor rgb="FF77F5F6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,40 +1098,40 @@
         <v>78</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -1914,40 +1920,40 @@
         <v>61</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="P16" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -1980,34 +1986,34 @@
         <v>94</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
@@ -2041,7 +2047,7 @@
         <v>95</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -2091,31 +2097,31 @@
         <v>63</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="O19" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="P19" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
@@ -2148,37 +2154,37 @@
         <v>96</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>64</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="P20" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
@@ -2207,7 +2213,7 @@
         <v>69</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -2339,7 +2345,7 @@
         <v>54</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -2389,58 +2395,58 @@
         <v>65</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="M25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="O25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="P25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="Q25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="R25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="S25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="T25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="U25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="V25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="W25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="X25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="Y25" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
@@ -2515,10 +2521,10 @@
         <v>99</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2891,31 +2897,31 @@
         <v>101</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="N35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="O35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="P35" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
@@ -3526,34 +3532,34 @@
         <v>90</v>
       </c>
       <c r="F46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="N46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O46" s="36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>

</xml_diff>